<commit_message>
backlog :D to write chosen tasks....
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maryam\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rassa.gh\Desktop\Soft_Lab_1\Census-Management-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>id</t>
   </si>
@@ -56,24 +56,108 @@
     <t>به عنوان کاربر برای یک کشور خاص که خودم انتخاب می‌کنم می‌خواهم تمام تخمین‌های رشد جمعیت را برای سال‌های مختلف در یک نمودار با رنگ‌های متفاوت ببینم در فایل پی‌دی‌اف.</t>
   </si>
   <si>
-    <t xml:space="preserve">به عنوان کاربر می‌خواهم لیست مرتب‌شده‌ی کشورها را برحسب میانگین نرخ سالانه‌ی رشد </t>
+    <t>به عنوان کاربر می‌خواهم لیست مرتب‌شده‌ی کشورها را برحسب میانگین نرخ سالانه‌ی رشد در یک بازه‌ی زمانی ببینم.</t>
+  </si>
+  <si>
+    <t>به عنوان کاربر می‌خواهم لیست مرتب‌شده‌ی کشورها را برحسب ماکسیمم میانگین نرخ سالانه‌ی رشد در بازه‌‌های زمانی مختلف ببینم.</t>
+  </si>
+  <si>
+    <t>انجام شد</t>
+  </si>
+  <si>
+    <t>تست نشده</t>
+  </si>
+  <si>
+    <t>گزارش</t>
+  </si>
+  <si>
+    <t>تست</t>
+  </si>
+  <si>
+    <t>کامل</t>
+  </si>
+  <si>
+    <t>باگ دارد</t>
+  </si>
+  <si>
+    <t>مرجش با اولی مونده</t>
+  </si>
+  <si>
+    <t>تخمین زمانی</t>
+  </si>
+  <si>
+    <t>تخمین زمانی جدید</t>
+  </si>
+  <si>
+    <t>مشکلات</t>
+  </si>
+  <si>
+    <t>تخمین زمانی اشتباه بوده</t>
+  </si>
+  <si>
+    <t>۱/۵ ساعت</t>
+  </si>
+  <si>
+    <t>۱۰ دقیقه</t>
+  </si>
+  <si>
+    <t>۱ ساعت</t>
+  </si>
+  <si>
+    <t>۴۵ دقیقه</t>
+  </si>
+  <si>
+    <t>۴۰ دقیقه</t>
+  </si>
+  <si>
+    <t>۲۰ دقیقه</t>
+  </si>
+  <si>
+    <t>۳۰ دقیقه</t>
+  </si>
+  <si>
+    <t>ناتمام</t>
+  </si>
+  <si>
+    <t>زمان واقعی</t>
+  </si>
+  <si>
+    <t>انجام دهنده</t>
+  </si>
+  <si>
+    <t>رسا</t>
+  </si>
+  <si>
+    <t>مریم</t>
+  </si>
+  <si>
+    <t>پردیس</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-3000000]dd\-mmm"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,12 +172,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -101,27 +209,88 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -396,99 +565,265 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="48" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="52.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.125" style="1"/>
-    <col min="4" max="4" width="12.25" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.125" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="12.28515625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="48" customHeight="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="48" customHeight="1">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" ht="48" customHeight="1">
+      <c r="A3" s="3">
+        <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" ht="48" customHeight="1">
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:A11" si="0">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="48" customHeight="1">
+      <c r="A5" s="3">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" ht="48" customHeight="1">
+      <c r="A6" s="3">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
+      <c r="C6" s="4">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" ht="48" customHeight="1">
+      <c r="A7" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" ht="48" customHeight="1">
+      <c r="A8" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" ht="48" customHeight="1">
+      <c r="A9" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" ht="48" customHeight="1">
+      <c r="A10" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" ht="48" customHeight="1">
+      <c r="A11" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="14" spans="1:8" ht="48" customHeight="1">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="19" spans="2:4" ht="48" customHeight="1">
+      <c r="B19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
task 6 was completed successfully... BUT! Strange diagrams! :(
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="48" customHeight="1"/>
@@ -743,7 +743,9 @@
       <c r="G7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="7"/>
+      <c r="H7" s="7">
+        <v>35</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="48" customHeight="1">
       <c r="A8" s="3">

</xml_diff>

<commit_message>
backlog was edited :D
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -568,7 +568,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="48" customHeight="1"/>
@@ -699,7 +699,9 @@
       <c r="G5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="7"/>
+      <c r="H5" s="7">
+        <v>90</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="48" customHeight="1">
       <c r="A6" s="3">

</xml_diff>

<commit_message>
bug fix test and burndownchart
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rassa.gh\Desktop\Soft_Lab_1\Census-Management-System\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pardis\Dropbox\[UNIVERSITY]\Sem8\Software Engineering Lab\Session 1\Census-Management-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10056" windowHeight="4632"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>id</t>
   </si>
@@ -132,14 +132,36 @@
   </si>
   <si>
     <t>پردیس</t>
+  </si>
+  <si>
+    <t>Task #</t>
+  </si>
+  <si>
+    <t>زمان تخمینی</t>
+  </si>
+  <si>
+    <t>روز ‍پایان</t>
+  </si>
+  <si>
+    <t>ساعت پایان</t>
+  </si>
+  <si>
+    <t>دقیقه پایان</t>
+  </si>
+  <si>
+    <t>دقیقه معادل</t>
+  </si>
+  <si>
+    <t>کار مانده</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-3000000]dd\-mmm"/>
+    <numFmt numFmtId="165" formatCode="[$-3000401]0"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -228,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -255,6 +277,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -300,6 +325,1170 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 2 Burndown Chart</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>actual</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Sheet1!$P$8,Sheet1!$P$2:$P$7,Sheet1!$P$9)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3590</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3760</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3775</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5570</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5720</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5880</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8640</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Sheet1!$Q$8,Sheet1!$Q$2:$Q$7,Sheet1!$Q$9)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0" formatCode="[$-3000401]0">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AB79-4155-BC87-96F48DE58F91}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>ideal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$8:$P$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8640</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$8:$Q$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="[$-3000401]0">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AB79-4155-BC87-96F48DE58F91}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="928126272"/>
+        <c:axId val="928131264"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="928126272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fa-IR"/>
+                  <a:t>زمان تا ددلاین (ساعت)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="928131264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="928131264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fa-IR"/>
+                  <a:t>کار لازم باقی مانده (ساعت)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="[$-3000401]0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="928126272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>87086</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>32658</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>315686</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>337458</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,6 +1567,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -413,6 +1619,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -565,22 +1788,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="48" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="48" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="52.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="12.28515625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="12.33203125" style="1" customWidth="1"/>
+    <col min="5" max="10" width="9.109375" style="1"/>
+    <col min="11" max="11" width="20.5546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.88671875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="48" customHeight="1">
+    <row r="1" spans="1:17" ht="48" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -605,8 +1833,29 @@
       <c r="H1" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="48" customHeight="1">
+    <row r="2" spans="1:17" ht="48" customHeight="1">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -627,8 +1876,31 @@
         <v>35</v>
       </c>
       <c r="H2" s="7"/>
+      <c r="K2" s="1">
+        <v>5</v>
+      </c>
+      <c r="L2" s="1">
+        <v>45</v>
+      </c>
+      <c r="M2" s="10">
+        <v>2</v>
+      </c>
+      <c r="N2" s="10">
+        <v>11</v>
+      </c>
+      <c r="O2" s="10">
+        <v>50</v>
+      </c>
+      <c r="P2" s="1">
+        <f>M2*24*60+N2*60+O2</f>
+        <v>3590</v>
+      </c>
+      <c r="Q2" s="1">
+        <f>265-L2</f>
+        <v>220</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" ht="48" customHeight="1">
+    <row r="3" spans="1:17" ht="48" customHeight="1">
       <c r="A3" s="3">
         <f>A2+1</f>
         <v>2</v>
@@ -651,11 +1923,36 @@
       <c r="G3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="7">
+        <v>170</v>
+      </c>
+      <c r="K3" s="1">
+        <v>7</v>
+      </c>
+      <c r="L3" s="1">
+        <v>20</v>
+      </c>
+      <c r="M3" s="1">
+        <v>2</v>
+      </c>
+      <c r="N3" s="1">
+        <v>14</v>
+      </c>
+      <c r="O3" s="1">
+        <v>40</v>
+      </c>
+      <c r="P3" s="1">
+        <f t="shared" ref="P3:P7" si="0">M3*24*60+N3*60+O3</f>
+        <v>3760</v>
+      </c>
+      <c r="Q3" s="1">
+        <f>Q2-L3</f>
+        <v>200</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" ht="48" customHeight="1">
+    <row r="4" spans="1:17" ht="48" customHeight="1">
       <c r="A4" s="3">
-        <f t="shared" ref="A4:A11" si="0">A3+1</f>
+        <f t="shared" ref="A4:A11" si="1">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -679,10 +1976,33 @@
       <c r="H4" s="7">
         <v>20</v>
       </c>
+      <c r="K4" s="1">
+        <v>2</v>
+      </c>
+      <c r="L4" s="1">
+        <v>90</v>
+      </c>
+      <c r="M4" s="1">
+        <v>2</v>
+      </c>
+      <c r="N4" s="1">
+        <v>14</v>
+      </c>
+      <c r="O4" s="1">
+        <v>55</v>
+      </c>
+      <c r="P4" s="1">
+        <f t="shared" si="0"/>
+        <v>3775</v>
+      </c>
+      <c r="Q4" s="1">
+        <f t="shared" ref="Q4:Q7" si="2">Q3-L4</f>
+        <v>110</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" ht="48" customHeight="1">
+    <row r="5" spans="1:17" ht="48" customHeight="1">
       <c r="A5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -702,10 +2022,33 @@
       <c r="H5" s="7">
         <v>90</v>
       </c>
+      <c r="K5" s="1">
+        <v>3</v>
+      </c>
+      <c r="L5" s="1">
+        <v>10</v>
+      </c>
+      <c r="M5" s="1">
+        <v>3</v>
+      </c>
+      <c r="N5" s="1">
+        <v>20</v>
+      </c>
+      <c r="O5" s="1">
+        <v>50</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="shared" si="0"/>
+        <v>5570</v>
+      </c>
+      <c r="Q5" s="1">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" ht="48" customHeight="1">
+    <row r="6" spans="1:17" ht="48" customHeight="1">
       <c r="A6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -726,11 +2069,36 @@
       <c r="G6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="7"/>
+      <c r="H6" s="7">
+        <v>20</v>
+      </c>
+      <c r="K6" s="1">
+        <v>6</v>
+      </c>
+      <c r="L6" s="1">
+        <v>40</v>
+      </c>
+      <c r="M6" s="1">
+        <v>3</v>
+      </c>
+      <c r="N6" s="1">
+        <v>23</v>
+      </c>
+      <c r="O6" s="1">
+        <v>20</v>
+      </c>
+      <c r="P6" s="1">
+        <f t="shared" si="0"/>
+        <v>5720</v>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" ht="48" customHeight="1">
+    <row r="7" spans="1:17" ht="48" customHeight="1">
       <c r="A7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -748,10 +2116,33 @@
       <c r="H7" s="7">
         <v>35</v>
       </c>
+      <c r="K7" s="1">
+        <v>4</v>
+      </c>
+      <c r="L7" s="1">
+        <v>60</v>
+      </c>
+      <c r="M7" s="1">
+        <v>4</v>
+      </c>
+      <c r="N7" s="1">
+        <v>2</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
+        <f t="shared" si="0"/>
+        <v>5880</v>
+      </c>
+      <c r="Q7" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" ht="48" customHeight="1">
+    <row r="8" spans="1:17" ht="48" customHeight="1">
       <c r="A8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -766,11 +2157,19 @@
       <c r="G8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="7"/>
+      <c r="H8" s="7">
+        <v>10</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>265</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" ht="48" customHeight="1">
+    <row r="9" spans="1:17" ht="48" customHeight="1">
       <c r="A9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -784,10 +2183,16 @@
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="7"/>
+      <c r="P9" s="1">
+        <v>8640</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:8" ht="48" customHeight="1">
+    <row r="10" spans="1:17" ht="48" customHeight="1">
       <c r="A10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -802,9 +2207,9 @@
       <c r="G10" s="6"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" ht="48" customHeight="1">
+    <row r="11" spans="1:17" ht="48" customHeight="1">
       <c r="A11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -819,7 +2224,7 @@
       <c r="G11" s="6"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="14" spans="1:8" ht="48" customHeight="1">
+    <row r="14" spans="1:17" ht="48" customHeight="1">
       <c r="D14" s="2"/>
     </row>
     <row r="19" spans="2:4" ht="48" customHeight="1">
@@ -833,5 +2238,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>